<commit_message>
se agrego relacion modelo de datos
</commit_message>
<xml_diff>
--- a/documentacion/modeloDatos.xlsx
+++ b/documentacion/modeloDatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SenaSoft\Desktop\senasoft\SenasoftGrupo2\documentatcion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SenaSoft\Desktop\senasoft\SenasoftGrupo2\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB8ED1BF-3AC2-4D15-B7C4-3361863D5445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963BECA4-5941-431E-8B8B-B80F6D3D0268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{3908351F-4F06-4FEB-A9BD-DC7C6B65D487}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3908351F-4F06-4FEB-A9BD-DC7C6B65D487}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>crra49</t>
+  </si>
+  <si>
+    <t>crra 90</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -244,6 +247,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -260,6 +266,336 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495303</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector: angular 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE8A6E76-3BA7-4F6A-A8AC-39ABBBB69A05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8701089" y="1119189"/>
+          <a:ext cx="2352675" cy="1809748"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2227"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>750752</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>132902</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector: angular 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1019B52-F180-4E6B-A4A9-AAEFB701C31F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7195500" y="2203952"/>
+          <a:ext cx="3580952" cy="1039948"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100272"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9527</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Conector: angular 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93A66B63-75FB-442C-90AA-7E45DB123E28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6886578" y="2524127"/>
+          <a:ext cx="4571996" cy="1371598"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Conector: angular 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F9CBC95-5191-4692-9897-3985DF35766B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6305552" y="2286002"/>
+          <a:ext cx="5534022" cy="2752725"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100258"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Conector: angular 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{494CB24F-2369-45D5-9820-8CEF26778EE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1790700" y="200025"/>
+          <a:ext cx="11953875" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -3705"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Conector recto de flecha 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A7F696-2CEB-4EAB-B6F2-5A994A760B2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13754100" y="180975"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,144 +895,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A42A4F-1C68-4FE2-8764-FA4B9C7DEC50}">
-  <dimension ref="B15:N30"/>
+  <dimension ref="B4:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="M4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="8">
+        <v>1010</v>
+      </c>
+      <c r="P7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>4</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>10</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="2">
-        <v>123456</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" s="2"/>
+      <c r="J18" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2">
+        <v>123456</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
         <v>2</v>
-      </c>
-      <c r="H19" s="2">
-        <v>20</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K19" s="2">
-        <v>98876</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="2">
+        <v>98876</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -705,86 +1133,54 @@
         <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N24" s="7"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>13</v>
+      <c r="C25" s="2">
+        <v>101</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3423432</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="H25" s="2">
-        <v>101</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K25" s="2">
-        <v>3423432</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" s="2">
-        <v>1</v>
-      </c>
-      <c r="N25" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
-        <v>2</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -793,103 +1189,123 @@
       <c r="M26" s="1"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>3</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="2">
-        <v>3</v>
-      </c>
-    </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
+      <c r="B28" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1010</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="2">
+        <v>453534</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2">
         <v>4</v>
       </c>
-      <c r="C28" s="5" t="s">
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2">
         <v>10</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1010</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="2">
-        <v>453534</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30" s="2">
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="2">
+        <v>2333</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C26" r:id="rId1" xr:uid="{EDE0B14E-2A0B-468B-90E0-1E0BBF94C604}"/>
-    <hyperlink ref="C27" r:id="rId2" xr:uid="{09CE80F5-CCD5-440B-A722-341C8E3B0A6A}"/>
-    <hyperlink ref="C25" r:id="rId3" xr:uid="{C1CD1ECC-CAAB-454B-95DA-91878D5A92D3}"/>
-    <hyperlink ref="C28" r:id="rId4" xr:uid="{B59557EA-CE16-4913-9A46-6FD68C090437}"/>
-    <hyperlink ref="C29" r:id="rId5" xr:uid="{B0642D49-4989-4F6B-B734-D3D7C9A5BF6F}"/>
+    <hyperlink ref="N7" r:id="rId1" xr:uid="{EDE0B14E-2A0B-468B-90E0-1E0BBF94C604}"/>
+    <hyperlink ref="N6" r:id="rId2" xr:uid="{C1CD1ECC-CAAB-454B-95DA-91878D5A92D3}"/>
+    <hyperlink ref="N8" r:id="rId3" xr:uid="{B59557EA-CE16-4913-9A46-6FD68C090437}"/>
+    <hyperlink ref="N10" r:id="rId4" xr:uid="{B0642D49-4989-4F6B-B734-D3D7C9A5BF6F}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{00BB0569-32E7-4DC5-9F24-18108FC4CFFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>